<commit_message>
add mux and adjust contril unit
</commit_message>
<xml_diff>
--- a/CPU-Guide/31连接表.xlsx
+++ b/CPU-Guide/31连接表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPU\StaticPipeline\CPU-Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C43CE7-0C2E-4ED2-9289-2B7858A16A08}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DF702D-2ECC-43F3-A65D-803E0F2C6E10}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2840" uniqueCount="139">
   <si>
     <t>表格 1</t>
   </si>
@@ -489,7 +489,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,6 +511,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -647,7 +653,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -684,44 +690,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -738,14 +711,53 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1909,11 +1921,11 @@
   </sheetPr>
   <dimension ref="A1:IV122"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="S54" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T66" sqref="T66:V66"/>
+      <selection pane="bottomRight" activeCell="AD2" sqref="AD2:AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1924,143 +1936,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="30.95" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="27"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="27"/>
+      <c r="AN1" s="27"/>
+      <c r="AO1" s="27"/>
+      <c r="AP1" s="27"/>
+      <c r="AQ1" s="27"/>
+      <c r="AR1" s="27"/>
+      <c r="AS1" s="27"/>
+      <c r="AT1" s="27"/>
+      <c r="AU1" s="27"/>
+      <c r="AV1" s="27"/>
+      <c r="AW1" s="27"/>
+      <c r="AX1" s="27"/>
+      <c r="AY1" s="27"/>
+      <c r="AZ1" s="27"/>
+      <c r="BA1" s="27"/>
+      <c r="BB1" s="27"/>
+      <c r="BC1" s="27"/>
+      <c r="BD1" s="27"/>
+      <c r="BE1" s="27"/>
+      <c r="BF1" s="27"/>
+      <c r="BG1" s="27"/>
     </row>
     <row r="2" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="13" t="s">
+      <c r="A2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="13" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="20" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="13" t="s">
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="13" t="s">
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="15"/>
-      <c r="T2" s="13" t="s">
+      <c r="S2" s="21"/>
+      <c r="T2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="13" t="s">
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="13" t="s">
+      <c r="X2" s="21"/>
+      <c r="Y2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="Z2" s="13" t="s">
+      <c r="Z2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="AA2" s="13" t="s">
+      <c r="AA2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="13" t="s">
+      <c r="AB2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="13" t="s">
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="AE2" s="13" t="s">
+      <c r="AE2" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="AF2" s="13" t="s">
+      <c r="AF2" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="AG2" s="13" t="s">
+      <c r="AG2" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="AH2" s="13" t="s">
+      <c r="AH2" s="33" t="s">
         <v>21</v>
       </c>
       <c r="HX2"/>
@@ -2090,17 +2102,17 @@
       <c r="IV2"/>
     </row>
     <row r="3" spans="1:256" ht="20.25" customHeight="1">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
@@ -2113,7 +2125,7 @@
       <c r="K3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="14"/>
+      <c r="L3" s="22"/>
       <c r="M3" s="3" t="s">
         <v>26</v>
       </c>
@@ -2150,20 +2162,20 @@
       <c r="X3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
       <c r="AB3" s="3" t="s">
         <v>37</v>
       </c>
       <c r="AC3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="14"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
+      <c r="AD3" s="34"/>
+      <c r="AE3" s="34"/>
+      <c r="AF3" s="34"/>
+      <c r="AG3" s="34"/>
+      <c r="AH3" s="34"/>
       <c r="HX3"/>
       <c r="HY3"/>
       <c r="HZ3"/>
@@ -2194,7 +2206,7 @@
       <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="12" t="s">
         <v>137</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -2278,7 +2290,7 @@
       <c r="IV4"/>
     </row>
     <row r="5" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -2361,7 +2373,7 @@
       <c r="IV5"/>
     </row>
     <row r="6" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A6" s="18"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="8" t="s">
         <v>50</v>
       </c>
@@ -2434,7 +2446,7 @@
       <c r="IV6"/>
     </row>
     <row r="7" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="23" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -2517,7 +2529,7 @@
       <c r="IV7"/>
     </row>
     <row r="8" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A8" s="18"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="8" t="s">
         <v>50</v>
       </c>
@@ -2590,7 +2602,7 @@
       <c r="IV8"/>
     </row>
     <row r="9" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="23" t="s">
         <v>55</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -2673,7 +2685,7 @@
       <c r="IV9"/>
     </row>
     <row r="10" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A10" s="18"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="8" t="s">
         <v>50</v>
       </c>
@@ -2746,7 +2758,7 @@
       <c r="IV10"/>
     </row>
     <row r="11" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="25" t="s">
         <v>59</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2829,7 +2841,7 @@
       <c r="IV11"/>
     </row>
     <row r="12" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A12" s="21"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="8" t="s">
         <v>64</v>
       </c>
@@ -2908,7 +2920,7 @@
       <c r="IV12"/>
     </row>
     <row r="13" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A13" s="21"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="8" t="s">
         <v>68</v>
       </c>
@@ -2977,7 +2989,7 @@
       <c r="IV13"/>
     </row>
     <row r="14" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="25" t="s">
         <v>70</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -3060,7 +3072,7 @@
       <c r="IV14"/>
     </row>
     <row r="15" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A15" s="21"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="8" t="s">
         <v>64</v>
       </c>
@@ -3139,7 +3151,7 @@
       <c r="IV15"/>
     </row>
     <row r="16" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A16" s="21"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="8" t="s">
         <v>68</v>
       </c>
@@ -3208,7 +3220,7 @@
       <c r="IV16"/>
     </row>
     <row r="17" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="23" t="s">
         <v>74</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -3285,7 +3297,7 @@
       <c r="IV17"/>
     </row>
     <row r="18" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A18" s="18"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="8" t="s">
         <v>50</v>
       </c>
@@ -3358,7 +3370,7 @@
       <c r="IV18"/>
     </row>
     <row r="19" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="23" t="s">
         <v>77</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -3441,7 +3453,7 @@
       <c r="IV19"/>
     </row>
     <row r="20" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A20" s="18"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="8" t="s">
         <v>72</v>
       </c>
@@ -3514,7 +3526,7 @@
       <c r="IV20"/>
     </row>
     <row r="21" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A21" s="18"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="8" t="s">
         <v>50</v>
       </c>
@@ -3587,7 +3599,7 @@
       <c r="IV21"/>
     </row>
     <row r="22" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="23" t="s">
         <v>79</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -3670,7 +3682,7 @@
       <c r="IV22"/>
     </row>
     <row r="23" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A23" s="18"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="8" t="s">
         <v>50</v>
       </c>
@@ -3743,7 +3755,7 @@
       <c r="IV23"/>
     </row>
     <row r="24" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="23" t="s">
         <v>82</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -3826,7 +3838,7 @@
       <c r="IV24"/>
     </row>
     <row r="25" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A25" s="18"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="8" t="s">
         <v>50</v>
       </c>
@@ -3899,7 +3911,7 @@
       <c r="IV25"/>
     </row>
     <row r="26" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="23" t="s">
         <v>85</v>
       </c>
       <c r="B26" s="8" t="s">
@@ -3982,7 +3994,7 @@
       <c r="IV26"/>
     </row>
     <row r="27" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A27" s="18"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="8" t="s">
         <v>50</v>
       </c>
@@ -4055,7 +4067,7 @@
       <c r="IV27"/>
     </row>
     <row r="28" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="23" t="s">
         <v>87</v>
       </c>
       <c r="B28" s="8" t="s">
@@ -4138,7 +4150,7 @@
       <c r="IV28"/>
     </row>
     <row r="29" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A29" s="18"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="8" t="s">
         <v>50</v>
       </c>
@@ -4211,7 +4223,7 @@
       <c r="IV29"/>
     </row>
     <row r="30" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="23" t="s">
         <v>90</v>
       </c>
       <c r="B30" s="8" t="s">
@@ -4294,7 +4306,7 @@
       <c r="IV30"/>
     </row>
     <row r="31" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A31" s="18"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="8" t="s">
         <v>50</v>
       </c>
@@ -4367,7 +4379,7 @@
       <c r="IV31"/>
     </row>
     <row r="32" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="13" t="s">
         <v>93</v>
       </c>
       <c r="B32" s="8" t="s">
@@ -4440,7 +4452,7 @@
       <c r="IV32"/>
     </row>
     <row r="33" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="25" t="s">
         <v>96</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -4515,7 +4527,7 @@
       <c r="IV33"/>
     </row>
     <row r="34" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A34" s="21"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="8" t="s">
         <v>68</v>
       </c>
@@ -4586,7 +4598,7 @@
       <c r="IV34"/>
     </row>
     <row r="35" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="23" t="s">
         <v>100</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -4669,7 +4681,7 @@
       <c r="IV35"/>
     </row>
     <row r="36" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A36" s="18"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="8" t="s">
         <v>50</v>
       </c>
@@ -4742,7 +4754,7 @@
       <c r="IV36"/>
     </row>
     <row r="37" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="23" t="s">
         <v>103</v>
       </c>
       <c r="B37" s="8" t="s">
@@ -4825,7 +4837,7 @@
       <c r="IV37"/>
     </row>
     <row r="38" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A38" s="18"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="8" t="s">
         <v>50</v>
       </c>
@@ -4898,7 +4910,7 @@
       <c r="IV38"/>
     </row>
     <row r="39" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="23" t="s">
         <v>104</v>
       </c>
       <c r="B39" s="8" t="s">
@@ -4981,7 +4993,7 @@
       <c r="IV39"/>
     </row>
     <row r="40" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A40" s="18"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="8" t="s">
         <v>50</v>
       </c>
@@ -5054,7 +5066,7 @@
       <c r="IV40"/>
     </row>
     <row r="41" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="13" t="s">
         <v>107</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -5127,7 +5139,7 @@
       <c r="IV41"/>
     </row>
     <row r="42" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="23" t="s">
         <v>108</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -5210,7 +5222,7 @@
       <c r="IV42"/>
     </row>
     <row r="43" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A43" s="18"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="8" t="s">
         <v>50</v>
       </c>
@@ -5283,7 +5295,7 @@
       <c r="IV43"/>
     </row>
     <row r="44" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="23" t="s">
         <v>111</v>
       </c>
       <c r="B44" s="8" t="s">
@@ -5366,7 +5378,7 @@
       <c r="IV44"/>
     </row>
     <row r="45" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A45" s="18"/>
+      <c r="A45" s="24"/>
       <c r="B45" s="8" t="s">
         <v>50</v>
       </c>
@@ -5439,7 +5451,7 @@
       <c r="IV45"/>
     </row>
     <row r="46" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="23" t="s">
         <v>113</v>
       </c>
       <c r="B46" s="8" t="s">
@@ -5522,7 +5534,7 @@
       <c r="IV46"/>
     </row>
     <row r="47" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A47" s="18"/>
+      <c r="A47" s="24"/>
       <c r="B47" s="8" t="s">
         <v>50</v>
       </c>
@@ -5595,7 +5607,7 @@
       <c r="IV47"/>
     </row>
     <row r="48" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="23" t="s">
         <v>117</v>
       </c>
       <c r="B48" s="8" t="s">
@@ -5678,7 +5690,7 @@
       <c r="IV48"/>
     </row>
     <row r="49" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A49" s="18"/>
+      <c r="A49" s="24"/>
       <c r="B49" s="8" t="s">
         <v>50</v>
       </c>
@@ -5751,7 +5763,7 @@
       <c r="IV49"/>
     </row>
     <row r="50" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="23" t="s">
         <v>119</v>
       </c>
       <c r="B50" s="8" t="s">
@@ -5834,7 +5846,7 @@
       <c r="IV50"/>
     </row>
     <row r="51" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A51" s="18"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="8" t="s">
         <v>50</v>
       </c>
@@ -5907,7 +5919,7 @@
       <c r="IV51"/>
     </row>
     <row r="52" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="23" t="s">
         <v>121</v>
       </c>
       <c r="B52" s="8" t="s">
@@ -5990,7 +6002,7 @@
       <c r="IV52"/>
     </row>
     <row r="53" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A53" s="18"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="8" t="s">
         <v>50</v>
       </c>
@@ -6063,7 +6075,7 @@
       <c r="IV53"/>
     </row>
     <row r="54" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="23" t="s">
         <v>122</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -6146,7 +6158,7 @@
       <c r="IV54"/>
     </row>
     <row r="55" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A55" s="18"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="8" t="s">
         <v>50</v>
       </c>
@@ -6219,7 +6231,7 @@
       <c r="IV55"/>
     </row>
     <row r="56" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="23" t="s">
         <v>125</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -6302,7 +6314,7 @@
       <c r="IV56"/>
     </row>
     <row r="57" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A57" s="18"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="8" t="s">
         <v>50</v>
       </c>
@@ -6375,7 +6387,7 @@
       <c r="IV57"/>
     </row>
     <row r="58" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="23" t="s">
         <v>127</v>
       </c>
       <c r="B58" s="8" t="s">
@@ -6458,7 +6470,7 @@
       <c r="IV58"/>
     </row>
     <row r="59" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A59" s="18"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="8" t="s">
         <v>50</v>
       </c>
@@ -6531,7 +6543,7 @@
       <c r="IV59"/>
     </row>
     <row r="60" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="23" t="s">
         <v>130</v>
       </c>
       <c r="B60" s="8" t="s">
@@ -6614,7 +6626,7 @@
       <c r="IV60"/>
     </row>
     <row r="61" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A61" s="18"/>
+      <c r="A61" s="24"/>
       <c r="B61" s="8" t="s">
         <v>50</v>
       </c>
@@ -6687,7 +6699,7 @@
       <c r="IV61"/>
     </row>
     <row r="62" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="23" t="s">
         <v>132</v>
       </c>
       <c r="B62" s="8" t="s">
@@ -6770,7 +6782,7 @@
       <c r="IV62"/>
     </row>
     <row r="63" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A63" s="18"/>
+      <c r="A63" s="24"/>
       <c r="B63" s="8" t="s">
         <v>50</v>
       </c>
@@ -6843,7 +6855,7 @@
       <c r="IV63"/>
     </row>
     <row r="64" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="23" t="s">
         <v>133</v>
       </c>
       <c r="B64" s="8" t="s">
@@ -6926,7 +6938,7 @@
       <c r="IV64"/>
     </row>
     <row r="65" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A65" s="18"/>
+      <c r="A65" s="24"/>
       <c r="B65" s="8" t="s">
         <v>50</v>
       </c>
@@ -6999,7 +7011,7 @@
       <c r="IV65"/>
     </row>
     <row r="66" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A66" s="17" t="s">
+      <c r="A66" s="23" t="s">
         <v>135</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -7082,7 +7094,7 @@
       <c r="IV66"/>
     </row>
     <row r="67" spans="1:256" ht="22.35" customHeight="1">
-      <c r="A67" s="18"/>
+      <c r="A67" s="24"/>
       <c r="B67" s="8" t="s">
         <v>50</v>
       </c>
@@ -7211,18 +7223,22 @@
     <row r="122" ht="22.35" customHeight="1"/>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A1:BG1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A62:A63"/>
     <mergeCell ref="A64:A65"/>
     <mergeCell ref="A66:A67"/>
@@ -7239,29 +7255,25 @@
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A44:A45"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A14:A16"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A1:BG1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="L2:L3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
@@ -7306,287 +7318,287 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="23" t="s">
+      <c r="A1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="31"/>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="23"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="29"/>
       <c r="J1" s="31"/>
       <c r="K1" s="31"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
       <c r="N1" s="31"/>
       <c r="O1" s="31"/>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
-      <c r="R1" s="23"/>
+      <c r="R1" s="29"/>
       <c r="S1" s="31"/>
-      <c r="T1" s="23"/>
+      <c r="T1" s="29"/>
       <c r="U1" s="31"/>
       <c r="V1" s="31"/>
-      <c r="W1" s="23"/>
+      <c r="W1" s="29"/>
       <c r="X1" s="31"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
       <c r="AC1" s="31"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="23"/>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23"/>
-      <c r="AN1" s="23"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
     </row>
     <row r="2" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="32" t="s">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
-      <c r="AI2" s="24"/>
-      <c r="AJ2" s="24"/>
-      <c r="AK2" s="24"/>
-      <c r="AL2" s="24"/>
-      <c r="AM2" s="24"/>
-      <c r="AN2" s="24"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="30"/>
+      <c r="AE2" s="30"/>
+      <c r="AF2" s="30"/>
+      <c r="AG2" s="30"/>
+      <c r="AH2" s="30"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="30"/>
+      <c r="AK2" s="30"/>
+      <c r="AL2" s="30"/>
+      <c r="AM2" s="30"/>
+      <c r="AN2" s="30"/>
     </row>
     <row r="3" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="14" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="17" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="14" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="14" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:40" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="15" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="14" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="14" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="15" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="14" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="14" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="14" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="14" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="14" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="14" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="14" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="14" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="14" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="14" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="14" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="14" t="s">
         <v>135</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AM1:AM2"/>
-    <mergeCell ref="AN1:AN2"/>
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
+    <mergeCell ref="AN1:AN2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7608,165 +7620,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="24"/>
+      <c r="A2" s="30"/>
     </row>
     <row r="3" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="14" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="17" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="14" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="14" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="15" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="14" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="14" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="15" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="14" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="14" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="14" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="14" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="14" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="14" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="14" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="14" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="14" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="14" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="14" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="14" t="s">
         <v>135</v>
       </c>
     </row>
@@ -7816,7 +7828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD65067-36B5-4773-945A-2DA6E46279FB}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B33" sqref="B33:D33"/>
     </sheetView>
   </sheetViews>
@@ -7829,17 +7841,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="24"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
@@ -7851,7 +7863,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="14" t="s">
         <v>138</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -7865,7 +7877,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="14" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -7879,7 +7891,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -7893,17 +7905,17 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="17" t="s">
         <v>74</v>
       </c>
       <c r="B8" s="9"/>
@@ -7915,7 +7927,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="17" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -7929,7 +7941,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="17" t="s">
         <v>79</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -7943,7 +7955,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="17" t="s">
         <v>82</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -7957,7 +7969,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>85</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -7971,7 +7983,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="14" t="s">
         <v>87</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -7985,7 +7997,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="14" t="s">
         <v>90</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -7999,17 +8011,17 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="15" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -8023,7 +8035,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="14" t="s">
         <v>103</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -8037,7 +8049,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="14" t="s">
         <v>104</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -8051,12 +8063,12 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="15" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="14" t="s">
         <v>108</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -8070,7 +8082,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="14" t="s">
         <v>111</v>
       </c>
       <c r="B22" s="10" t="s">
@@ -8084,7 +8096,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="14" t="s">
         <v>113</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -8098,7 +8110,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="14" t="s">
         <v>117</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -8112,7 +8124,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="14" t="s">
         <v>119</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -8126,7 +8138,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="14" t="s">
         <v>121</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -8140,7 +8152,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="14" t="s">
         <v>122</v>
       </c>
       <c r="B27" s="10" t="s">
@@ -8154,7 +8166,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="14" t="s">
         <v>125</v>
       </c>
       <c r="B28" s="10" t="s">
@@ -8168,7 +8180,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="14" t="s">
         <v>127</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -8182,7 +8194,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="14" t="s">
         <v>130</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -8196,7 +8208,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="14" t="s">
         <v>132</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -8210,7 +8222,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -8224,7 +8236,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="14" t="s">
         <v>135</v>
       </c>
       <c r="B33" s="10" t="s">
@@ -8297,17 +8309,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="24"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="3" t="s">
         <v>24</v>
       </c>
@@ -8319,37 +8331,37 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="14" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="17" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="17" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -8361,22 +8373,22 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="14" t="s">
         <v>87</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -8390,102 +8402,102 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="14" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="15" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="14" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="14" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="15" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="14" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="14" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="14" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="14" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="14" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="14" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="14" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="14" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="14" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="14" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="14" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="14" t="s">
         <v>135</v>
       </c>
     </row>
@@ -8549,17 +8561,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="24"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
@@ -8571,7 +8583,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="14" t="s">
         <v>138</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -8585,7 +8597,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="14" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -8599,7 +8611,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -8613,17 +8625,17 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="17" t="s">
         <v>74</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -8637,7 +8649,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="17" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -8651,7 +8663,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="17" t="s">
         <v>79</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -8665,7 +8677,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="17" t="s">
         <v>82</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -8679,7 +8691,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="14" t="s">
         <v>85</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -8693,12 +8705,12 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="14" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="14" t="s">
         <v>90</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -8712,17 +8724,17 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="15" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -8736,7 +8748,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="14" t="s">
         <v>103</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -8750,7 +8762,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="14" t="s">
         <v>104</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -8764,12 +8776,12 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="15" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="14" t="s">
         <v>108</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -8783,7 +8795,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="14" t="s">
         <v>111</v>
       </c>
       <c r="B22" s="10" t="s">
@@ -8797,7 +8809,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="14" t="s">
         <v>113</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -8811,7 +8823,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="14" t="s">
         <v>117</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -8825,7 +8837,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="14" t="s">
         <v>119</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -8839,7 +8851,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="14" t="s">
         <v>121</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -8853,7 +8865,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="14" t="s">
         <v>122</v>
       </c>
       <c r="B27" s="10" t="s">
@@ -8867,7 +8879,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="14" t="s">
         <v>125</v>
       </c>
       <c r="B28" s="10" t="s">
@@ -8881,7 +8893,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="14" t="s">
         <v>127</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -8895,7 +8907,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="14" t="s">
         <v>130</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -8909,7 +8921,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="14" t="s">
         <v>132</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -8923,7 +8935,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -8937,7 +8949,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="14" t="s">
         <v>135</v>
       </c>
       <c r="B33" s="10" t="s">
@@ -8990,5 +9002,6 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add ID Control Unit
</commit_message>
<xml_diff>
--- a/CPU-Guide/31连接表.xlsx
+++ b/CPU-Guide/31连接表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPU\StaticPipeline\CPU-Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DF702D-2ECC-43F3-A65D-803E0F2C6E10}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F27B35-F2EA-4CBC-921C-AD49073B366B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2840" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="139">
   <si>
     <t>表格 1</t>
   </si>
@@ -1921,8 +1921,8 @@
   </sheetPr>
   <dimension ref="A1:IV122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="AD2" sqref="AD2:AH3"/>
@@ -8297,7 +8297,7 @@
   <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:D13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>